<commit_message>
Untested but test passing, EPUB code
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/multipage-bad-sequence/manifest.xlsx
+++ b/spec/fixtures/files/multipage-bad-sequence/manifest.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beekerz/Documents/cerberus/spec/fixtures/files/multipage-bad-sequence/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nakatomi/Projects/Vagrant/drs-v1/spec/fixtures/files/multipage-bad-sequence/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AAE33C-B338-E743-A507-E83FDF0A5359}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="460" windowWidth="25000" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="1280" yWindow="1080" windowWidth="25000" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -113,6 +114,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -380,11 +384,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,7 +441,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
@@ -451,7 +455,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>

</xml_diff>